<commit_message>
added more good quality samples
</commit_message>
<xml_diff>
--- a/Data/tensile test.xlsx
+++ b/Data/tensile test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanzhouf\Documents\GitHub\Dataset-in-situ-monitoring-FFF-structures\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7464D8C-6E6B-4DCD-A159-845AF3E1152A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDD36F3-0C10-4DAE-A1BE-EC3E37838E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="570" windowWidth="10650" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1323,9 +1323,6 @@
     <t>LINE1L2.5L357P6</t>
   </si>
   <si>
-    <t>LINE1L4.5L24P5</t>
-  </si>
-  <si>
     <t>LINE1L06L3P15</t>
   </si>
   <si>
@@ -1510,6 +1507,9 @@
   </si>
   <si>
     <t>good47</t>
+  </si>
+  <si>
+    <t>LINE1L4.5L2P5</t>
   </si>
 </sst>
 </file>
@@ -1855,47 +1855,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A429" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C451" sqref="C451"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
     <col min="5" max="5" width="7.140625" customWidth="1"/>
     <col min="6" max="6" width="5.85546875" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
-    <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
-    <col min="16" max="16" width="17" customWidth="1"/>
-    <col min="17" max="17" width="0.28515625" customWidth="1"/>
-    <col min="18" max="18" width="0.5703125" customWidth="1"/>
-    <col min="19" max="19" width="0.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="0.140625" customWidth="1"/>
+    <col min="10" max="10" width="2" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="13" width="9.85546875" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" customWidth="1"/>
+    <col min="17" max="17" width="0.5703125" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="0.42578125" customWidth="1"/>
     <col min="20" max="20" width="13.5703125" customWidth="1"/>
     <col min="21" max="21" width="10.7109375" customWidth="1"/>
-    <col min="22" max="22" width="15" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" customWidth="1"/>
     <col min="23" max="23" width="12" customWidth="1"/>
     <col min="24" max="24" width="9.7109375" customWidth="1"/>
-    <col min="25" max="25" width="7.140625" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="0.140625" customWidth="1"/>
-    <col min="27" max="27" width="5" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="0.7109375" customWidth="1"/>
+    <col min="26" max="26" width="13.28515625" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="0.28515625" customWidth="1"/>
     <col min="28" max="28" width="17.7109375" customWidth="1"/>
     <col min="30" max="30" width="14" customWidth="1"/>
     <col min="31" max="31" width="19.5703125" customWidth="1"/>
-    <col min="32" max="32" width="13.42578125" customWidth="1"/>
-    <col min="33" max="33" width="0.7109375" customWidth="1"/>
-    <col min="34" max="34" width="0.5703125" customWidth="1"/>
-    <col min="35" max="35" width="1.140625" customWidth="1"/>
-    <col min="36" max="36" width="11.140625" customWidth="1"/>
+    <col min="32" max="32" width="15.42578125" customWidth="1"/>
+    <col min="33" max="34" width="0.28515625" customWidth="1"/>
+    <col min="35" max="35" width="0.7109375" customWidth="1"/>
+    <col min="36" max="36" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="17.25" x14ac:dyDescent="0.25">
@@ -50207,10 +50205,10 @@
         <v>410</v>
       </c>
       <c r="C385">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D385" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E385">
         <v>2</v>
@@ -50272,57 +50270,56 @@
         <v>0</v>
       </c>
       <c r="V385">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="W385">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X385">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Y385">
         <f t="shared" si="80"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z385">
         <f t="shared" si="81"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AA385">
         <f t="shared" si="82"/>
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="AB385" s="4">
         <f t="shared" si="83"/>
-        <v>10.04987562112089</v>
+        <v>0</v>
       </c>
       <c r="AC385">
         <v>0</v>
       </c>
       <c r="AD385">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="AE385">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF385">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AG385">
         <f t="shared" si="84"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH385">
-        <f t="shared" si="85"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AI385">
         <f t="shared" si="86"/>
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="AJ385" s="4">
         <f t="shared" si="87"/>
-        <v>10.04987562112089</v>
+        <v>0</v>
       </c>
     </row>
     <row r="386" spans="1:36" x14ac:dyDescent="0.25">
@@ -50496,85 +50493,82 @@
         <v>0</v>
       </c>
       <c r="N387">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="O387">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P387">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q387">
         <f t="shared" ref="Q387:R414" si="91">O387^2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R387">
-        <f t="shared" si="91"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S387">
         <f t="shared" ref="S387:S414" si="92">Q387+R387</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T387" s="4">
         <f t="shared" ref="T387:T414" si="93">SQRT(S387)</f>
-        <v>1.4142135623730951</v>
+        <v>0</v>
       </c>
       <c r="U387">
         <v>0</v>
       </c>
       <c r="V387">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="W387">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X387">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y387">
         <f t="shared" ref="Y387:Z414" si="94">W387^2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z387">
-        <f t="shared" si="94"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA387">
         <f t="shared" ref="AA387:AA414" si="95">Y387+Z387</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB387" s="4">
         <f t="shared" ref="AB387:AB414" si="96">SQRT(AA387)</f>
-        <v>1.4142135623730951</v>
+        <v>0</v>
       </c>
       <c r="AC387">
         <v>0</v>
       </c>
       <c r="AD387">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="AE387">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF387">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG387">
         <f t="shared" ref="AG387:AH414" si="97">AE387^2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH387">
-        <f t="shared" si="97"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI387">
         <f t="shared" ref="AI387:AI414" si="98">AG387+AH387</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AJ387" s="4">
         <f t="shared" ref="AJ387:AJ414" si="99">SQRT(AI387)</f>
-        <v>1.4142135623730951</v>
+        <v>0</v>
       </c>
     </row>
     <row r="388" spans="1:36" x14ac:dyDescent="0.25">
@@ -50585,10 +50579,10 @@
         <v>413</v>
       </c>
       <c r="C388">
-        <v>869</v>
+        <v>950</v>
       </c>
       <c r="D388" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="E388">
         <v>3</v>
@@ -50678,29 +50672,28 @@
         <v>0</v>
       </c>
       <c r="AD388">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="AE388">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF388">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AG388">
         <f t="shared" si="97"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH388">
-        <f t="shared" si="97"/>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="AI388">
         <f t="shared" si="98"/>
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="AJ388" s="4">
         <f t="shared" si="99"/>
-        <v>6.0827625302982193</v>
+        <v>0</v>
       </c>
     </row>
     <row r="389" spans="1:36" x14ac:dyDescent="0.25">
@@ -50708,13 +50701,13 @@
         <v>388</v>
       </c>
       <c r="B389" t="s">
-        <v>414</v>
+        <v>476</v>
       </c>
       <c r="C389">
-        <v>924</v>
+        <v>938</v>
       </c>
       <c r="D389" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E389">
         <v>2</v>
@@ -50745,88 +50738,85 @@
         <v>5.0990195135927845</v>
       </c>
       <c r="M389">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N389">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="O389">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P389">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q389">
         <f t="shared" si="91"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R389">
         <f t="shared" si="91"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="S389">
         <f t="shared" si="92"/>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="T389" s="4">
-        <f t="shared" si="93"/>
-        <v>5.0990195135927845</v>
+        <v>0</v>
       </c>
       <c r="U389">
         <v>0</v>
       </c>
       <c r="V389">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="W389">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X389">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Y389">
         <f t="shared" si="94"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z389">
         <f t="shared" si="94"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AA389">
         <f t="shared" si="95"/>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AB389" s="4">
-        <f t="shared" si="96"/>
-        <v>5.0990195135927845</v>
+        <v>0</v>
       </c>
       <c r="AC389">
         <v>0</v>
       </c>
       <c r="AD389">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="AE389">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF389">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AG389">
         <f t="shared" si="97"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH389">
         <f t="shared" si="97"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AI389">
         <f t="shared" si="98"/>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AJ389" s="4">
-        <f t="shared" si="99"/>
-        <v>5.0990195135927845</v>
+        <v>0</v>
       </c>
     </row>
     <row r="390" spans="1:36" x14ac:dyDescent="0.25">
@@ -50834,7 +50824,7 @@
         <v>389</v>
       </c>
       <c r="B390" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C390">
         <v>941</v>
@@ -50874,85 +50864,82 @@
         <v>0</v>
       </c>
       <c r="N390">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O390">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P390">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Q390">
         <f t="shared" si="91"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R390">
-        <f t="shared" si="91"/>
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="S390">
         <f t="shared" si="92"/>
-        <v>226</v>
+        <v>0</v>
       </c>
       <c r="T390" s="4">
         <f t="shared" si="93"/>
-        <v>15.033296378372908</v>
+        <v>0</v>
       </c>
       <c r="U390">
         <v>0</v>
       </c>
       <c r="V390">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="W390">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X390">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Y390">
         <f t="shared" si="94"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z390">
-        <f t="shared" si="94"/>
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="AA390">
         <f t="shared" si="95"/>
-        <v>226</v>
+        <v>0</v>
       </c>
       <c r="AB390" s="4">
         <f t="shared" si="96"/>
-        <v>15.033296378372908</v>
+        <v>0</v>
       </c>
       <c r="AC390">
         <v>0</v>
       </c>
       <c r="AD390">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AE390">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF390">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AG390">
         <f t="shared" si="97"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH390">
-        <f t="shared" si="97"/>
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="AI390">
         <f t="shared" si="98"/>
-        <v>226</v>
+        <v>0</v>
       </c>
       <c r="AJ390" s="4">
         <f t="shared" si="99"/>
-        <v>15.033296378372908</v>
+        <v>0</v>
       </c>
     </row>
     <row r="391" spans="1:36" x14ac:dyDescent="0.25">
@@ -50960,7 +50947,7 @@
         <v>390</v>
       </c>
       <c r="B391" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C391">
         <v>935</v>
@@ -51000,85 +50987,84 @@
         <v>0</v>
       </c>
       <c r="N391">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="O391">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P391">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="Q391">
         <f t="shared" si="91"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R391">
-        <f t="shared" si="91"/>
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="S391">
         <f t="shared" si="92"/>
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="T391" s="4">
         <f t="shared" si="93"/>
-        <v>12.041594578792296</v>
+        <v>0</v>
       </c>
       <c r="U391">
         <v>0</v>
       </c>
       <c r="V391">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="W391">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X391">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="Y391">
         <f t="shared" si="94"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z391">
         <f t="shared" si="94"/>
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="AA391">
         <f t="shared" si="95"/>
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="AB391" s="4">
         <f t="shared" si="96"/>
-        <v>12.041594578792296</v>
+        <v>0</v>
       </c>
       <c r="AC391">
         <v>0</v>
       </c>
       <c r="AD391">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="AE391">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF391">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AG391">
         <f t="shared" si="97"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH391">
         <f t="shared" si="97"/>
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="AI391">
         <f t="shared" si="98"/>
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="AJ391" s="4">
         <f t="shared" si="99"/>
-        <v>12.041594578792296</v>
+        <v>0</v>
       </c>
     </row>
     <row r="392" spans="1:36" x14ac:dyDescent="0.25">
@@ -51086,7 +51072,7 @@
         <v>391</v>
       </c>
       <c r="B392" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C392">
         <v>919</v>
@@ -51126,85 +51112,82 @@
         <v>0</v>
       </c>
       <c r="N392">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="O392">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P392">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Q392">
         <f t="shared" si="91"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R392">
-        <f t="shared" si="91"/>
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="S392">
         <f t="shared" si="92"/>
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="T392" s="4">
         <f t="shared" si="93"/>
-        <v>9.0553851381374173</v>
+        <v>0</v>
       </c>
       <c r="U392">
         <v>0</v>
       </c>
       <c r="V392">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="W392">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X392">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Y392">
         <f t="shared" si="94"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z392">
-        <f t="shared" si="94"/>
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="AA392">
         <f t="shared" si="95"/>
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="AB392" s="4">
         <f t="shared" si="96"/>
-        <v>9.0553851381374173</v>
+        <v>0</v>
       </c>
       <c r="AC392">
         <v>0</v>
       </c>
       <c r="AD392">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="AE392">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF392">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AG392">
         <f t="shared" si="97"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH392">
-        <f t="shared" si="97"/>
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="AI392">
         <f t="shared" si="98"/>
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="AJ392" s="4">
         <f t="shared" si="99"/>
-        <v>9.0553851381374173</v>
+        <v>0</v>
       </c>
     </row>
     <row r="393" spans="1:36" x14ac:dyDescent="0.25">
@@ -51212,7 +51195,7 @@
         <v>392</v>
       </c>
       <c r="B393" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C393">
         <v>942</v>
@@ -51252,85 +51235,83 @@
         <v>0</v>
       </c>
       <c r="N393">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O393">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P393">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q393">
         <f t="shared" si="91"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R393">
-        <f t="shared" si="91"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="S393">
         <f t="shared" si="92"/>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T393" s="4">
         <f t="shared" si="93"/>
-        <v>4.1231056256176606</v>
+        <v>0</v>
       </c>
       <c r="U393">
         <v>0</v>
       </c>
       <c r="V393">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="W393">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X393">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Y393">
         <f t="shared" si="94"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z393">
-        <f t="shared" si="94"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AA393">
         <f t="shared" si="95"/>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="AB393" s="4">
         <f t="shared" si="96"/>
-        <v>4.1231056256176606</v>
+        <v>0</v>
       </c>
       <c r="AC393">
         <v>0</v>
       </c>
       <c r="AD393">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AE393">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF393">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AG393">
         <f t="shared" si="97"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH393">
         <f t="shared" si="97"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AI393">
         <f t="shared" si="98"/>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="AJ393" s="4">
         <f t="shared" si="99"/>
-        <v>4.1231056256176606</v>
+        <v>0</v>
       </c>
     </row>
     <row r="394" spans="1:36" x14ac:dyDescent="0.25">
@@ -51338,7 +51319,7 @@
         <v>393</v>
       </c>
       <c r="B394" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C394">
         <v>920</v>
@@ -51406,57 +51387,57 @@
         <v>0</v>
       </c>
       <c r="V394">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="W394">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X394">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="Y394">
         <f t="shared" si="94"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z394">
         <f t="shared" si="94"/>
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="AA394">
         <f t="shared" si="95"/>
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="AB394" s="4">
         <f t="shared" si="96"/>
-        <v>12.041594578792296</v>
+        <v>0</v>
       </c>
       <c r="AC394">
         <v>0</v>
       </c>
       <c r="AD394">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AE394">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF394">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AG394">
         <f t="shared" si="97"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH394">
         <f t="shared" si="97"/>
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="AI394">
         <f t="shared" si="98"/>
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="AJ394" s="4">
         <f t="shared" si="99"/>
-        <v>12.041594578792296</v>
+        <v>0</v>
       </c>
     </row>
     <row r="395" spans="1:36" x14ac:dyDescent="0.25">
@@ -51464,7 +51445,7 @@
         <v>394</v>
       </c>
       <c r="B395" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C395">
         <v>933</v>
@@ -51504,85 +51485,82 @@
         <v>0</v>
       </c>
       <c r="N395">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="O395">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P395">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q395">
         <f t="shared" si="91"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R395">
-        <f t="shared" si="91"/>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="S395">
         <f t="shared" si="92"/>
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="T395" s="4">
         <f t="shared" si="93"/>
-        <v>6.0827625302982193</v>
+        <v>0</v>
       </c>
       <c r="U395">
         <v>0</v>
       </c>
       <c r="V395">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="W395">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X395">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Y395">
         <f t="shared" si="94"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z395">
-        <f t="shared" si="94"/>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="AA395">
         <f t="shared" si="95"/>
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="AB395" s="4">
         <f t="shared" si="96"/>
-        <v>6.0827625302982193</v>
+        <v>0</v>
       </c>
       <c r="AC395">
         <v>0</v>
       </c>
       <c r="AD395">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="AE395">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF395">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AG395">
         <f t="shared" si="97"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH395">
         <f t="shared" si="97"/>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="AI395">
-        <f t="shared" si="98"/>
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="AJ395" s="4">
         <f t="shared" si="99"/>
-        <v>6.0827625302982193</v>
+        <v>0</v>
       </c>
     </row>
     <row r="396" spans="1:36" x14ac:dyDescent="0.25">
@@ -51590,7 +51568,7 @@
         <v>395</v>
       </c>
       <c r="B396" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C396">
         <v>908</v>
@@ -51686,29 +51664,29 @@
         <v>0</v>
       </c>
       <c r="AD396">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AE396">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF396">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AG396">
         <f t="shared" si="97"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH396">
         <f t="shared" si="97"/>
-        <v>144</v>
+        <v>0</v>
       </c>
       <c r="AI396">
         <f t="shared" si="98"/>
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="AJ396" s="4">
         <f t="shared" si="99"/>
-        <v>12.041594578792296</v>
+        <v>0</v>
       </c>
     </row>
     <row r="397" spans="1:36" x14ac:dyDescent="0.25">
@@ -51716,10 +51694,10 @@
         <v>396</v>
       </c>
       <c r="B397" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C397">
-        <v>932</v>
+        <v>949</v>
       </c>
       <c r="D397" t="s">
         <v>406</v>
@@ -51812,29 +51790,28 @@
         <v>0</v>
       </c>
       <c r="AD397">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="AE397">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF397">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AG397">
         <f t="shared" si="97"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH397">
-        <f t="shared" si="97"/>
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="AI397">
         <f t="shared" si="98"/>
-        <v>229</v>
+        <v>0</v>
       </c>
       <c r="AJ397" s="4">
         <f t="shared" si="99"/>
-        <v>15.132745950421556</v>
+        <v>0</v>
       </c>
     </row>
     <row r="398" spans="1:36" x14ac:dyDescent="0.25">
@@ -51842,7 +51819,7 @@
         <v>397</v>
       </c>
       <c r="B398" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C398">
         <v>951</v>
@@ -51910,57 +51887,57 @@
         <v>0</v>
       </c>
       <c r="V398">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="W398">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X398">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Y398">
         <f t="shared" si="94"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z398">
         <f t="shared" si="94"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AA398">
         <f t="shared" si="95"/>
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="AB398" s="4">
         <f t="shared" si="96"/>
-        <v>10.198039027185569</v>
+        <v>0</v>
       </c>
       <c r="AC398">
         <v>0</v>
       </c>
       <c r="AD398">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="AE398">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF398">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AG398">
         <f t="shared" si="97"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH398">
         <f t="shared" si="97"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AI398">
         <f t="shared" si="98"/>
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="AJ398" s="4">
         <f t="shared" si="99"/>
-        <v>10.198039027185569</v>
+        <v>0</v>
       </c>
     </row>
     <row r="399" spans="1:36" x14ac:dyDescent="0.25">
@@ -51968,7 +51945,7 @@
         <v>398</v>
       </c>
       <c r="B399" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C399">
         <v>964</v>
@@ -52008,85 +51985,85 @@
         <v>0</v>
       </c>
       <c r="N399">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="O399">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P399">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q399">
         <f t="shared" si="91"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R399">
         <f t="shared" si="91"/>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="S399">
         <f t="shared" si="92"/>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="T399" s="4">
         <f t="shared" si="93"/>
-        <v>6.324555320336759</v>
+        <v>0</v>
       </c>
       <c r="U399">
         <v>0</v>
       </c>
       <c r="V399">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="W399">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X399">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Y399">
         <f t="shared" si="94"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z399">
         <f t="shared" si="94"/>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="AA399">
         <f t="shared" si="95"/>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AB399" s="4">
         <f t="shared" si="96"/>
-        <v>6.324555320336759</v>
+        <v>0</v>
       </c>
       <c r="AC399">
         <v>0</v>
       </c>
       <c r="AD399">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="AE399">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF399">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AG399">
         <f t="shared" si="97"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH399">
         <f t="shared" si="97"/>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="AI399">
         <f t="shared" si="98"/>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AJ399" s="4">
         <f t="shared" si="99"/>
-        <v>6.324555320336759</v>
+        <v>0</v>
       </c>
     </row>
     <row r="400" spans="1:36" x14ac:dyDescent="0.25">
@@ -52094,7 +52071,7 @@
         <v>399</v>
       </c>
       <c r="B400" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C400">
         <v>953</v>
@@ -52162,57 +52139,56 @@
         <v>0</v>
       </c>
       <c r="V400">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="W400">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X400">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Y400">
         <f t="shared" si="94"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z400">
         <f t="shared" si="94"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AA400">
         <f t="shared" si="95"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AB400" s="4">
         <f t="shared" si="96"/>
-        <v>4.4721359549995796</v>
+        <v>0</v>
       </c>
       <c r="AC400">
         <v>0</v>
       </c>
       <c r="AD400">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="AE400">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF400">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AG400">
         <f t="shared" si="97"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH400">
         <f t="shared" si="97"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AI400">
-        <f t="shared" si="98"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AJ400" s="4">
         <f t="shared" si="99"/>
-        <v>4.4721359549995796</v>
+        <v>0</v>
       </c>
     </row>
     <row r="401" spans="1:36" x14ac:dyDescent="0.25">
@@ -52220,7 +52196,7 @@
         <v>400</v>
       </c>
       <c r="B401" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C401">
         <v>902</v>
@@ -52316,29 +52292,29 @@
         <v>0</v>
       </c>
       <c r="AD401">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="AE401">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF401">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AG401">
         <f t="shared" si="97"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH401">
         <f t="shared" si="97"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AI401">
         <f t="shared" si="98"/>
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="AJ401" s="4">
         <f t="shared" si="99"/>
-        <v>10.198039027185569</v>
+        <v>0</v>
       </c>
     </row>
     <row r="402" spans="1:36" x14ac:dyDescent="0.25">
@@ -52346,7 +52322,7 @@
         <v>401</v>
       </c>
       <c r="B402" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C402">
         <v>941</v>
@@ -52414,57 +52390,57 @@
         <v>0</v>
       </c>
       <c r="V402">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="W402">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X402">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Y402">
         <f t="shared" si="94"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z402">
         <f t="shared" si="94"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AA402">
         <f t="shared" si="95"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AB402" s="4">
         <f t="shared" si="96"/>
-        <v>4.4721359549995796</v>
+        <v>0</v>
       </c>
       <c r="AC402">
         <v>0</v>
       </c>
       <c r="AD402">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="AE402">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF402">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AG402">
         <f t="shared" si="97"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH402">
         <f t="shared" si="97"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AI402">
         <f t="shared" si="98"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AJ402" s="4">
         <f t="shared" si="99"/>
-        <v>4.4721359549995796</v>
+        <v>0</v>
       </c>
     </row>
     <row r="403" spans="1:36" x14ac:dyDescent="0.25">
@@ -52472,7 +52448,7 @@
         <v>402</v>
       </c>
       <c r="B403" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C403">
         <v>907</v>
@@ -52540,57 +52516,57 @@
         <v>0</v>
       </c>
       <c r="V403">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="W403">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X403">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="Y403">
         <f t="shared" si="94"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z403">
         <f t="shared" si="94"/>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="AA403">
         <f t="shared" si="95"/>
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="AB403" s="4">
         <f t="shared" si="96"/>
-        <v>8.2462112512353212</v>
+        <v>0</v>
       </c>
       <c r="AC403">
         <v>0</v>
       </c>
       <c r="AD403">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AE403">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF403">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AG403">
         <f t="shared" si="97"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH403">
         <f t="shared" si="97"/>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="AI403">
         <f t="shared" si="98"/>
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="AJ403" s="4">
         <f t="shared" si="99"/>
-        <v>8.2462112512353212</v>
+        <v>0</v>
       </c>
     </row>
     <row r="404" spans="1:36" x14ac:dyDescent="0.25">
@@ -52598,7 +52574,7 @@
         <v>403</v>
       </c>
       <c r="B404" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C404">
         <v>937</v>
@@ -52638,85 +52614,85 @@
         <v>0</v>
       </c>
       <c r="N404">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O404">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P404">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q404">
         <f t="shared" si="91"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R404">
         <f t="shared" si="91"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="S404">
         <f t="shared" si="92"/>
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="T404" s="4">
         <f t="shared" si="93"/>
-        <v>5.3851648071345037</v>
+        <v>0</v>
       </c>
       <c r="U404">
         <v>0</v>
       </c>
       <c r="V404">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="W404">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X404">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Y404">
         <f t="shared" si="94"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z404">
         <f t="shared" si="94"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AA404">
         <f t="shared" si="95"/>
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="AB404" s="4">
         <f t="shared" si="96"/>
-        <v>5.3851648071345037</v>
+        <v>0</v>
       </c>
       <c r="AC404">
         <v>0</v>
       </c>
       <c r="AD404">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AE404">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF404">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AG404">
         <f t="shared" si="97"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH404">
         <f t="shared" si="97"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AI404">
         <f t="shared" si="98"/>
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="AJ404" s="4">
         <f t="shared" si="99"/>
-        <v>5.3851648071345037</v>
+        <v>0</v>
       </c>
     </row>
     <row r="405" spans="1:36" x14ac:dyDescent="0.25">
@@ -52724,7 +52700,7 @@
         <v>404</v>
       </c>
       <c r="B405" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C405">
         <v>940</v>
@@ -52792,57 +52768,56 @@
         <v>0</v>
       </c>
       <c r="V405">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="W405">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X405">
         <v>6</v>
       </c>
       <c r="Y405">
         <f t="shared" si="94"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z405">
-        <f t="shared" si="94"/>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="AA405">
         <f t="shared" si="95"/>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AB405" s="4">
         <f t="shared" si="96"/>
-        <v>6.324555320336759</v>
+        <v>0</v>
       </c>
       <c r="AC405">
         <v>0</v>
       </c>
       <c r="AD405">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AE405">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF405">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AG405">
         <f t="shared" si="97"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH405">
         <f t="shared" si="97"/>
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="AI405">
         <f t="shared" si="98"/>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AJ405" s="4">
         <f t="shared" si="99"/>
-        <v>6.324555320336759</v>
+        <v>0</v>
       </c>
     </row>
     <row r="406" spans="1:36" x14ac:dyDescent="0.25">
@@ -52850,7 +52825,7 @@
         <v>405</v>
       </c>
       <c r="B406" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C406">
         <v>920</v>
@@ -52893,82 +52868,82 @@
         <v>14</v>
       </c>
       <c r="O406">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P406">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Q406">
         <f t="shared" si="91"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R406">
         <f t="shared" si="91"/>
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="S406">
         <f t="shared" si="92"/>
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="T406" s="4">
         <f t="shared" si="93"/>
-        <v>9.2195444572928871</v>
+        <v>0</v>
       </c>
       <c r="U406">
         <v>0</v>
       </c>
       <c r="V406">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="W406">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X406">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Y406">
         <f t="shared" si="94"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Z406">
         <f t="shared" si="94"/>
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="AA406">
         <f t="shared" si="95"/>
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="AB406" s="4">
         <f t="shared" si="96"/>
-        <v>9.2195444572928871</v>
+        <v>0</v>
       </c>
       <c r="AC406">
         <v>0</v>
       </c>
       <c r="AD406">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="AE406">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF406">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AG406">
         <f t="shared" si="97"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH406">
         <f t="shared" si="97"/>
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="AI406">
         <f t="shared" si="98"/>
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="AJ406" s="4">
         <f t="shared" si="99"/>
-        <v>9.2195444572928871</v>
+        <v>0</v>
       </c>
     </row>
     <row r="407" spans="1:36" x14ac:dyDescent="0.25">
@@ -52976,7 +52951,7 @@
         <v>406</v>
       </c>
       <c r="B407" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C407">
         <v>956</v>
@@ -53072,29 +53047,29 @@
         <v>0</v>
       </c>
       <c r="AD407">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="AE407">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF407">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AG407">
         <f t="shared" si="97"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AH407">
         <f t="shared" si="97"/>
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="AI407">
         <f t="shared" si="98"/>
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="AJ407" s="4">
         <f t="shared" si="99"/>
-        <v>7.6157731058639087</v>
+        <v>0</v>
       </c>
     </row>
     <row r="408" spans="1:36" x14ac:dyDescent="0.25">
@@ -53102,7 +53077,7 @@
         <v>407</v>
       </c>
       <c r="B408" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C408">
         <v>950</v>
@@ -53170,57 +53145,57 @@
         <v>0</v>
       </c>
       <c r="V408">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="W408">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X408">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y408">
         <f t="shared" si="94"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Z408">
         <f t="shared" si="94"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AA408">
         <f t="shared" si="95"/>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="AB408" s="4">
         <f t="shared" si="96"/>
-        <v>3.6055512754639891</v>
+        <v>0</v>
       </c>
       <c r="AC408">
         <v>0</v>
       </c>
       <c r="AD408">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="AE408">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF408">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG408">
         <f t="shared" si="97"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AH408">
         <f t="shared" si="97"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AI408">
         <f t="shared" si="98"/>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="AJ408" s="4">
         <f t="shared" si="99"/>
-        <v>3.6055512754639891</v>
+        <v>0</v>
       </c>
     </row>
     <row r="409" spans="1:36" x14ac:dyDescent="0.25">
@@ -53228,7 +53203,7 @@
         <v>408</v>
       </c>
       <c r="B409" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C409">
         <v>945</v>
@@ -53324,29 +53299,28 @@
         <v>0</v>
       </c>
       <c r="AD409">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="AE409">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF409">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AG409">
         <f t="shared" si="97"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AH409">
         <f t="shared" si="97"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AI409">
-        <f t="shared" si="98"/>
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="AJ409" s="4">
         <f t="shared" si="99"/>
-        <v>10.440306508910551</v>
+        <v>0</v>
       </c>
     </row>
     <row r="410" spans="1:36" x14ac:dyDescent="0.25">
@@ -53354,10 +53328,10 @@
         <v>409</v>
       </c>
       <c r="B410" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C410">
-        <v>902</v>
+        <v>932</v>
       </c>
       <c r="D410" t="s">
         <v>406</v>
@@ -53394,85 +53368,84 @@
         <v>0</v>
       </c>
       <c r="N410">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="O410">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P410">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q410">
         <f t="shared" si="91"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="R410">
         <f t="shared" si="91"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="S410">
         <f t="shared" si="92"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="T410" s="4">
         <f t="shared" si="93"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U410">
         <v>0</v>
       </c>
       <c r="V410">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="W410">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X410">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Y410">
         <f t="shared" si="94"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Z410">
-        <f t="shared" si="94"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AA410">
         <f t="shared" si="95"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AB410" s="4">
         <f t="shared" si="96"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AC410">
         <v>0</v>
       </c>
       <c r="AD410">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="AE410">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF410">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AG410">
         <f t="shared" si="97"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AH410">
         <f t="shared" si="97"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="AI410">
         <f t="shared" si="98"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AJ410" s="4">
         <f t="shared" si="99"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="411" spans="1:36" x14ac:dyDescent="0.25">
@@ -53480,7 +53453,7 @@
         <v>410</v>
       </c>
       <c r="B411" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C411">
         <v>903</v>
@@ -53576,29 +53549,29 @@
         <v>0</v>
       </c>
       <c r="AD411">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="AE411">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF411">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AG411">
         <f t="shared" si="97"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AH411">
         <f t="shared" si="97"/>
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="AI411">
         <f t="shared" si="98"/>
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="AJ411" s="4">
         <f t="shared" si="99"/>
-        <v>7.6157731058639087</v>
+        <v>0</v>
       </c>
     </row>
     <row r="412" spans="1:36" x14ac:dyDescent="0.25">
@@ -53606,7 +53579,7 @@
         <v>411</v>
       </c>
       <c r="B412" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C412">
         <v>917</v>
@@ -53674,57 +53647,57 @@
         <v>0</v>
       </c>
       <c r="V412">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="W412">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X412">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="Y412">
         <f t="shared" si="94"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Z412">
         <f t="shared" si="94"/>
-        <v>169</v>
+        <v>0</v>
       </c>
       <c r="AA412">
         <f t="shared" si="95"/>
-        <v>178</v>
+        <v>0</v>
       </c>
       <c r="AB412" s="4">
         <f t="shared" si="96"/>
-        <v>13.341664064126334</v>
+        <v>0</v>
       </c>
       <c r="AC412">
         <v>0</v>
       </c>
       <c r="AD412">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AE412">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF412">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="AG412">
         <f t="shared" si="97"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AH412">
         <f t="shared" si="97"/>
-        <v>169</v>
+        <v>0</v>
       </c>
       <c r="AI412">
         <f t="shared" si="98"/>
-        <v>178</v>
+        <v>0</v>
       </c>
       <c r="AJ412" s="4">
         <f t="shared" si="99"/>
-        <v>13.341664064126334</v>
+        <v>0</v>
       </c>
     </row>
     <row r="413" spans="1:36" x14ac:dyDescent="0.25">
@@ -53732,7 +53705,7 @@
         <v>412</v>
       </c>
       <c r="B413" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C413">
         <v>913</v>
@@ -53828,29 +53801,29 @@
         <v>0</v>
       </c>
       <c r="AD413">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AE413">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF413">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AG413">
         <f t="shared" si="97"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AH413">
         <f t="shared" si="97"/>
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="AI413">
         <f t="shared" si="98"/>
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="AJ413" s="4">
         <f t="shared" si="99"/>
-        <v>7.6157731058639087</v>
+        <v>0</v>
       </c>
     </row>
     <row r="414" spans="1:36" x14ac:dyDescent="0.25">
@@ -53858,7 +53831,7 @@
         <v>413</v>
       </c>
       <c r="B414" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C414">
         <v>938</v>
@@ -53898,85 +53871,84 @@
         <v>0</v>
       </c>
       <c r="N414">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="O414">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P414">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Q414">
         <f t="shared" si="91"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="R414">
         <f t="shared" si="91"/>
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="S414">
         <f t="shared" si="92"/>
-        <v>234</v>
+        <v>0</v>
       </c>
       <c r="T414" s="4">
         <f t="shared" si="93"/>
-        <v>15.297058540778355</v>
+        <v>0</v>
       </c>
       <c r="U414">
         <v>0</v>
       </c>
       <c r="V414">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="W414">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="X414">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Y414">
         <f t="shared" si="94"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Z414">
         <f t="shared" si="94"/>
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="AA414">
         <f t="shared" si="95"/>
-        <v>234</v>
+        <v>0</v>
       </c>
       <c r="AB414" s="4">
         <f t="shared" si="96"/>
-        <v>15.297058540778355</v>
+        <v>0</v>
       </c>
       <c r="AC414">
         <v>0</v>
       </c>
       <c r="AD414">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="AE414">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF414">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AG414">
         <f t="shared" si="97"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AH414">
         <f t="shared" si="97"/>
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="AI414">
-        <f t="shared" si="98"/>
-        <v>234</v>
+        <v>0</v>
       </c>
       <c r="AJ414" s="4">
         <f t="shared" si="99"/>
-        <v>15.297058540778355</v>
+        <v>0</v>
       </c>
     </row>
     <row r="415" spans="1:36" x14ac:dyDescent="0.25">
@@ -53984,7 +53956,7 @@
         <v>414</v>
       </c>
       <c r="B415" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C415">
         <v>966</v>
@@ -54094,7 +54066,7 @@
         <v>415</v>
       </c>
       <c r="B416" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C416">
         <v>963</v>
@@ -54204,7 +54176,7 @@
         <v>416</v>
       </c>
       <c r="B417" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C417">
         <v>973</v>
@@ -54314,7 +54286,7 @@
         <v>417</v>
       </c>
       <c r="B418" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C418">
         <v>970</v>
@@ -54424,7 +54396,7 @@
         <v>418</v>
       </c>
       <c r="B419" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C419">
         <v>968</v>
@@ -54534,7 +54506,7 @@
         <v>419</v>
       </c>
       <c r="B420" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C420">
         <v>979</v>
@@ -54644,7 +54616,7 @@
         <v>420</v>
       </c>
       <c r="B421" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C421">
         <v>965</v>
@@ -54754,7 +54726,7 @@
         <v>421</v>
       </c>
       <c r="B422" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C422">
         <v>977</v>
@@ -54864,7 +54836,7 @@
         <v>422</v>
       </c>
       <c r="B423" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C423">
         <v>976</v>
@@ -54974,7 +54946,7 @@
         <v>423</v>
       </c>
       <c r="B424" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C424">
         <v>975</v>
@@ -55084,7 +55056,7 @@
         <v>424</v>
       </c>
       <c r="B425" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C425">
         <v>968</v>
@@ -55194,7 +55166,7 @@
         <v>425</v>
       </c>
       <c r="B426" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C426">
         <v>971</v>
@@ -55304,7 +55276,7 @@
         <v>426</v>
       </c>
       <c r="B427" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C427">
         <v>974</v>
@@ -55414,7 +55386,7 @@
         <v>427</v>
       </c>
       <c r="B428" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C428">
         <v>985</v>
@@ -55524,7 +55496,7 @@
         <v>428</v>
       </c>
       <c r="B429" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C429">
         <v>972</v>
@@ -55634,7 +55606,7 @@
         <v>429</v>
       </c>
       <c r="B430" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C430">
         <v>970</v>
@@ -55744,7 +55716,7 @@
         <v>430</v>
       </c>
       <c r="B431" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C431">
         <v>970</v>
@@ -55854,7 +55826,7 @@
         <v>431</v>
       </c>
       <c r="B432" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C432">
         <v>973</v>
@@ -55964,7 +55936,7 @@
         <v>432</v>
       </c>
       <c r="B433" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C433">
         <v>966</v>
@@ -56074,7 +56046,7 @@
         <v>433</v>
       </c>
       <c r="B434" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C434">
         <v>979</v>
@@ -56184,7 +56156,7 @@
         <v>434</v>
       </c>
       <c r="B435" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C435">
         <v>980</v>
@@ -56294,7 +56266,7 @@
         <v>435</v>
       </c>
       <c r="B436" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C436">
         <v>961</v>
@@ -56404,7 +56376,7 @@
         <v>436</v>
       </c>
       <c r="B437" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C437">
         <v>977</v>
@@ -56514,7 +56486,7 @@
         <v>437</v>
       </c>
       <c r="B438" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C438">
         <v>968</v>
@@ -56624,7 +56596,7 @@
         <v>438</v>
       </c>
       <c r="B439" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C439">
         <v>970</v>
@@ -56734,7 +56706,7 @@
         <v>439</v>
       </c>
       <c r="B440" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C440">
         <v>966</v>
@@ -56844,7 +56816,7 @@
         <v>440</v>
       </c>
       <c r="B441" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C441">
         <v>970</v>
@@ -56954,7 +56926,7 @@
         <v>441</v>
       </c>
       <c r="B442" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C442">
         <v>973</v>
@@ -57064,7 +57036,7 @@
         <v>442</v>
       </c>
       <c r="B443" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C443">
         <v>969</v>
@@ -57174,7 +57146,7 @@
         <v>443</v>
       </c>
       <c r="B444" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C444">
         <v>969</v>
@@ -57284,7 +57256,7 @@
         <v>444</v>
       </c>
       <c r="B445" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C445">
         <v>975</v>
@@ -57394,7 +57366,7 @@
         <v>445</v>
       </c>
       <c r="B446" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C446">
         <v>977</v>
@@ -57504,7 +57476,7 @@
         <v>446</v>
       </c>
       <c r="B447" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C447">
         <v>969</v>
@@ -57614,7 +57586,7 @@
         <v>447</v>
       </c>
       <c r="B448" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C448">
         <v>972</v>
@@ -57724,7 +57696,7 @@
         <v>448</v>
       </c>
       <c r="B449" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C449">
         <v>979</v>
@@ -57834,7 +57806,7 @@
         <v>449</v>
       </c>
       <c r="B450" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C450">
         <v>980</v>
@@ -57944,7 +57916,7 @@
         <v>450</v>
       </c>
       <c r="B451" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C451">
         <v>971</v>

</xml_diff>